<commit_message>
Aufgabenliste und Fragen geändert
</commit_message>
<xml_diff>
--- a/Aufgabenliste für Projekte1.xlsx
+++ b/Aufgabenliste für Projekte1.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHIARA\OneDrive\PSE\Git\PSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joana\OneDrive\Dokumente\GitHub\PSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="E13436A57EBF1EF23878CA726A73DCB28D344F81" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{A412F747-F542-45AC-BE60-6052FF3130DD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabenliste" sheetId="1" r:id="rId1"/>
-    <sheet name="Ideen_Probleme" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprache" sheetId="3" r:id="rId3"/>
+    <sheet name="Fragen" sheetId="4" r:id="rId2"/>
+    <sheet name="Ideen_Probleme" sheetId="2" r:id="rId3"/>
+    <sheet name="Sprache" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Aufgabenliste!$B$5:$B$37</definedName>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="114">
   <si>
     <t>Aufgabenliste</t>
   </si>
@@ -346,11 +348,38 @@
   <si>
     <t>a</t>
   </si>
+  <si>
+    <t>7. /14. fürs Pflichtenheft nachschauen</t>
+  </si>
+  <si>
+    <t>Joana</t>
+  </si>
+  <si>
+    <t>8. fürs Pflichtenheft nachschauen</t>
+  </si>
+  <si>
+    <t>Bene</t>
+  </si>
+  <si>
+    <t>Skizze für GUI</t>
+  </si>
+  <si>
+    <t>11. Systemmodelle nachschauen &amp; 13</t>
+  </si>
+  <si>
+    <t>Programm zum durchlaufen von Programmen</t>
+  </si>
+  <si>
+    <t>Systemmodelle: UML/Sequenzdiagamme normalerweiße Entwurf?</t>
+  </si>
+  <si>
+    <t>Idee für Trace (Antler funktioniert nicht mit Rückgängig machen)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -598,7 +627,6 @@
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -699,6 +727,7 @@
     <xf numFmtId="14" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1080,47 +1109,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.1796875" style="2"/>
-    <col min="2" max="2" width="10.08984375" style="2"/>
-    <col min="3" max="3" width="22.26953125" style="2"/>
-    <col min="4" max="4" width="10.54296875" style="2"/>
-    <col min="5" max="5" width="23.7265625" style="2"/>
-    <col min="6" max="6" width="9" style="2"/>
-    <col min="7" max="7" width="19.54296875" style="2"/>
-    <col min="8" max="8" width="5.6328125" style="2"/>
-    <col min="9" max="9" width="10.81640625" style="2"/>
-    <col min="10" max="10" width="9" style="2"/>
-    <col min="11" max="11" width="27.08984375" style="2"/>
-    <col min="12" max="1025" width="9" style="2"/>
+    <col min="1" max="1" width="1.21875" style="1"/>
+    <col min="2" max="2" width="10.109375" style="1"/>
+    <col min="3" max="3" width="22.21875" style="1"/>
+    <col min="4" max="4" width="10.5546875" style="1"/>
+    <col min="5" max="5" width="23.77734375" style="1"/>
+    <col min="6" max="6" width="9" style="1"/>
+    <col min="7" max="7" width="19.5546875" style="1"/>
+    <col min="8" max="8" width="5.6640625" style="1"/>
+    <col min="9" max="9" width="10.77734375" style="1"/>
+    <col min="10" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="27.109375" style="1"/>
+    <col min="12" max="1025" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="41.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1024" ht="41.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="43"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="L1"/>
@@ -2143,10 +2172,10 @@
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>43178</v>
       </c>
       <c r="H2"/>
@@ -3167,12 +3196,12 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" ht="15.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3"/>
@@ -4197,7 +4226,7 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -5223,50 +5252,50 @@
       <c r="AMI4"/>
       <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1024" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:1024" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="I5" s="12" t="s">
+      <c r="G5" s="10"/>
+      <c r="I5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
       <c r="H6"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="6" t="s">
+      <c r="J6" s="20"/>
+      <c r="K6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="L6"/>
@@ -6285,26 +6314,26 @@
     </row>
     <row r="7" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>43045</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
       <c r="H7"/>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="L7"/>
@@ -7323,26 +7352,26 @@
     </row>
     <row r="8" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="26">
         <v>43045</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
       <c r="H8"/>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L8"/>
@@ -8361,21 +8390,21 @@
     </row>
     <row r="9" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>43047</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="29"/>
       <c r="H9"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
       <c r="L9"/>
       <c r="M9"/>
       <c r="N9"/>
@@ -9392,24 +9421,24 @@
     </row>
     <row r="10" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>43057</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
       <c r="H10"/>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="2" t="s">
+      <c r="J10" s="20"/>
+      <c r="K10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L10"/>
@@ -10428,26 +10457,26 @@
     </row>
     <row r="11" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <v>43061</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
       <c r="H11"/>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L11"/>
@@ -11466,24 +11495,24 @@
     </row>
     <row r="12" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <v>43063</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
       <c r="H12"/>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="2" t="s">
+      <c r="J12" s="20"/>
+      <c r="K12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="L12"/>
@@ -12502,26 +12531,26 @@
     </row>
     <row r="13" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="26">
         <v>43064</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
       <c r="H13"/>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="L13"/>
@@ -13540,20 +13569,20 @@
     </row>
     <row r="14" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
       <c r="H14"/>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="2" t="s">
+      <c r="J14" s="20"/>
+      <c r="K14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="L14"/>
@@ -14572,18 +14601,22 @@
     </row>
     <row r="15" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
       <c r="H15"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
-      <c r="K15"/>
+      <c r="I15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="20"/>
+      <c r="K15" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="L15"/>
       <c r="M15"/>
       <c r="N15"/>
@@ -15602,14 +15635,18 @@
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
-      <c r="D16" s="36"/>
+      <c r="D16" s="35"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="21"/>
-      <c r="K16"/>
+      <c r="I16" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="L16"/>
       <c r="M16"/>
       <c r="N16"/>
@@ -16624,42 +16661,51 @@
       <c r="AMI16"/>
       <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1:1024" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="1:1024" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="21"/>
+      <c r="G17" s="10"/>
+      <c r="I17" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="18" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="38" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="38">
         <v>43068</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
       <c r="H18"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21"/>
-      <c r="K18"/>
+      <c r="I18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="L18"/>
       <c r="M18"/>
       <c r="N18"/>
@@ -17676,18 +17722,22 @@
     </row>
     <row r="19" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="22" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
       <c r="H19"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21"/>
-      <c r="K19"/>
+      <c r="I19" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="L19"/>
       <c r="M19"/>
       <c r="N19"/>
@@ -18704,17 +18754,17 @@
     </row>
     <row r="20" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="30"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
       <c r="H20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="21"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
@@ -19732,17 +19782,17 @@
     </row>
     <row r="21" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="22" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="26"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
       <c r="H21"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
@@ -20760,17 +20810,17 @@
     </row>
     <row r="22" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
       <c r="H22"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
@@ -21788,17 +21838,17 @@
     </row>
     <row r="23" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="22" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
       <c r="H23"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
       <c r="K23"/>
       <c r="L23"/>
       <c r="M23"/>
@@ -22816,17 +22866,17 @@
     </row>
     <row r="24" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15" t="s">
+      <c r="B24" s="13"/>
+      <c r="C24" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="30"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
       <c r="H24"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="21"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
       <c r="K24"/>
       <c r="L24"/>
       <c r="M24"/>
@@ -23844,17 +23894,17 @@
     </row>
     <row r="25" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="22" t="s">
+      <c r="B25" s="13"/>
+      <c r="C25" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25"/>
       <c r="H25"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="21"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
@@ -24872,17 +24922,17 @@
     </row>
     <row r="26" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="31" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
       <c r="H26"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="21"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="20"/>
       <c r="K26"/>
       <c r="L26"/>
       <c r="M26"/>
@@ -25900,15 +25950,15 @@
     </row>
     <row r="27" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
-      <c r="B27" s="40"/>
+      <c r="B27" s="39"/>
       <c r="C27"/>
-      <c r="D27" s="36"/>
+      <c r="D27" s="35"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="21"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="20"/>
       <c r="K27"/>
       <c r="L27"/>
       <c r="M27"/>
@@ -26924,117 +26974,117 @@
       <c r="AMI27"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="13" t="s">
+    <row r="28" spans="1:1024" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="11"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="21"/>
+      <c r="G28" s="10"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="14"/>
-      <c r="C29" s="38" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="19"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="21"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
-      <c r="C30" s="22" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="14"/>
-      <c r="C31" s="38" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="41"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
     </row>
     <row r="32" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="14"/>
-      <c r="C32" s="22" t="s">
+      <c r="B32" s="13"/>
+      <c r="C32" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="26"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="14"/>
-      <c r="C33" s="38" t="s">
+      <c r="B33" s="13"/>
+      <c r="C33" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
     </row>
     <row r="34" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="14"/>
-      <c r="C34" s="22" t="s">
+      <c r="B34" s="13"/>
+      <c r="C34" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
     </row>
     <row r="35" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14"/>
-      <c r="C35" s="38" t="s">
+      <c r="B35" s="13"/>
+      <c r="C35" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29"/>
     </row>
     <row r="36" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="14"/>
-      <c r="C36" s="22" t="s">
+      <c r="B36" s="13"/>
+      <c r="C36" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="26"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="25"/>
     </row>
     <row r="37" spans="2:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="14"/>
-      <c r="C37" s="34" t="s">
+      <c r="B37" s="13"/>
+      <c r="C37" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="35"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="34"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38"/>
@@ -27045,112 +27095,112 @@
       <c r="G38"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G39" s="11"/>
+      <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B40" s="14"/>
-      <c r="C40" s="38" t="s">
+    <row r="40" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B40" s="13"/>
+      <c r="C40" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="39"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="19"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="18"/>
     </row>
-    <row r="41" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="14"/>
-      <c r="C41" s="22" t="s">
+    <row r="41" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B41" s="13"/>
+      <c r="C41" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="26"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="25"/>
     </row>
-    <row r="42" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="14"/>
-      <c r="C42" s="38" t="s">
+    <row r="42" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B42" s="13"/>
+      <c r="C42" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="30"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29"/>
     </row>
-    <row r="43" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="14"/>
-      <c r="C43" s="22" t="s">
+    <row r="43" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B43" s="13"/>
+      <c r="C43" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="23"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="26"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="25"/>
     </row>
-    <row r="44" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="14"/>
-      <c r="C44" s="38" t="s">
+    <row r="44" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B44" s="13"/>
+      <c r="C44" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="30"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="29"/>
     </row>
-    <row r="45" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="14"/>
-      <c r="C45" s="22" t="s">
+    <row r="45" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B45" s="13"/>
+      <c r="C45" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="26"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="25"/>
     </row>
-    <row r="46" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B46" s="14"/>
-      <c r="C46" s="38" t="s">
+    <row r="46" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B46" s="13"/>
+      <c r="C46" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="30"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="29"/>
     </row>
-    <row r="47" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="14"/>
-      <c r="C47" s="22" t="s">
+    <row r="47" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B47" s="13"/>
+      <c r="C47" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="25"/>
     </row>
-    <row r="48" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B48" s="14"/>
-      <c r="C48" s="34" t="s">
+    <row r="48" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B48" s="13"/>
+      <c r="C48" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D48" s="42"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="35"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="34"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49"/>
@@ -27161,115 +27211,115 @@
       <c r="G49"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="37" t="s">
+      <c r="D50" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G50" s="11"/>
+      <c r="G50" s="10"/>
     </row>
-    <row r="51" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B51" s="14"/>
-      <c r="C51" s="38" t="s">
+    <row r="51" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B51" s="13"/>
+      <c r="C51" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="39"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="19"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
     </row>
-    <row r="52" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B52" s="14"/>
-      <c r="C52" s="22" t="s">
+    <row r="52" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B52" s="13"/>
+      <c r="C52" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="26"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="25"/>
     </row>
-    <row r="53" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="14"/>
-      <c r="C53" s="38" t="s">
+    <row r="53" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B53" s="13"/>
+      <c r="C53" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D53" s="41"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="30"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="29"/>
     </row>
-    <row r="54" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B54" s="14"/>
-      <c r="C54" s="22" t="s">
+    <row r="54" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B54" s="13"/>
+      <c r="C54" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="26"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="25"/>
     </row>
-    <row r="55" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B55" s="14"/>
-      <c r="C55" s="38" t="s">
+    <row r="55" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B55" s="13"/>
+      <c r="C55" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="41"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="30"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="29"/>
     </row>
-    <row r="56" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B56" s="14"/>
-      <c r="C56" s="22" t="s">
+    <row r="56" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B56" s="13"/>
+      <c r="C56" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="26"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="25"/>
     </row>
-    <row r="57" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B57" s="14"/>
-      <c r="C57" s="38" t="s">
+    <row r="57" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B57" s="13"/>
+      <c r="C57" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D57" s="41"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="30"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="29"/>
     </row>
-    <row r="58" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B58" s="14"/>
-      <c r="C58" s="22" t="s">
+    <row r="58" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B58" s="13"/>
+      <c r="C58" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D58" s="23"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="26"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="25"/>
     </row>
-    <row r="59" spans="2:7" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B59" s="14"/>
-      <c r="C59" s="34" t="s">
+    <row r="59" spans="2:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B59" s="13"/>
+      <c r="C59" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D59" s="42"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="35"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="34"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:B37"/>
+  <autoFilter ref="B5:B37" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
@@ -27279,182 +27329,274 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE6AD51-2E4D-4100-BE95-FF351D40D03B}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="58.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+    </row>
+    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+    </row>
+    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+    </row>
+    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+    </row>
+    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+    </row>
+    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+    </row>
+    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+    </row>
+    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+    </row>
+    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+    </row>
+    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+    </row>
+    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+    </row>
+    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+    </row>
+    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+    </row>
+    <row r="17" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+    </row>
+    <row r="18" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+    </row>
+    <row r="19" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+    </row>
+    <row r="20" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+    </row>
+    <row r="21" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+    </row>
+    <row r="22" spans="1:1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="10.54296875"/>
+    <col min="1" max="1025" width="10.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="42" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="42" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="42" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="42" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="43" t="s">
+      <c r="J7" s="42" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="J8" s="42" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="42" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="43" t="s">
+      <c r="J10" s="42" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="43" t="s">
+      <c r="J11" s="42" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="43" t="s">
+      <c r="J12" s="42" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="42" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="42" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="42" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="42" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="42" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="42" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="42" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="42" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="42" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="42" t="s">
         <v>85</v>
       </c>
     </row>
@@ -27464,78 +27606,78 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="10.54296875"/>
+    <col min="1" max="1025" width="10.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="42" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="42" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="42" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="42" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="42" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="42" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="42" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="42" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>